<commit_message>
paropakar final and dhikurepati final
</commit_message>
<xml_diff>
--- a/ofc/estimates/lakilla mandir/lakilla mandir.xlsx
+++ b/ofc/estimates/lakilla mandir/lakilla mandir.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\lakilla mandir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\lakilla mandir\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WCR" sheetId="6" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">estimate!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -351,10 +351,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -586,7 +586,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -596,7 +596,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -618,7 +618,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -634,7 +634,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -643,7 +643,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -652,7 +652,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -671,7 +671,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -703,7 +703,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -724,7 +724,7 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -742,84 +742,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="22" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="21" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -835,6 +768,73 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1261,107 +1261,107 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="75" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="77" t="s">
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="72" t="e">
+      <c r="C6" s="76" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="73"/>
+      <c r="D6" s="77"/>
       <c r="E6" s="11"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -1369,13 +1369,13 @@
         <v>18</v>
       </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="72" t="e">
+      <c r="J6" s="76" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="73"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="77"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>27</v>
       </c>
@@ -1384,75 +1384,75 @@
       <c r="D7" s="12"/>
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
-      <c r="I7" s="68" t="s">
+      <c r="I7" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="67" t="e">
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="84" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="I8" s="69" t="s">
+      <c r="B8" s="84"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
+      <c r="I8" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="70" t="e">
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="87" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="70"/>
-      <c r="I9" s="69" t="s">
+      <c r="B9" s="87"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="I9" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="65" t="s">
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="71" t="s">
+      <c r="D11" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71" t="s">
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="65" t="s">
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="66" t="s">
+      <c r="K11" s="83" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="65"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="82"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
       <c r="D12" s="13" t="s">
         <v>24</v>
       </c>
@@ -1471,10 +1471,10 @@
       <c r="I12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="65"/>
-      <c r="K12" s="66"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="82"/>
+      <c r="K12" s="83"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="K13" s="17"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
       <c r="B14" s="36" t="e">
         <f>#REF!</f>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="K14" s="17"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="36"/>
       <c r="C15" s="14"/>
@@ -1555,7 +1555,7 @@
       <c r="J15" s="34"/>
       <c r="K15" s="17"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="K16" s="17"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" s="35"/>
       <c r="C17" s="14"/>
@@ -1611,7 +1611,7 @@
       <c r="J17" s="34"/>
       <c r="K17" s="17"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>15</v>
@@ -1637,13 +1637,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -1656,6 +1649,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1673,105 +1673,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F160" sqref="F160"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="M139" sqref="M139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="83" t="s">
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-    </row>
-    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="84" t="s">
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
         <v>46</v>
       </c>
@@ -1781,31 +1781,31 @@
       <c r="E6" s="42"/>
       <c r="F6" s="42"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="81" t="s">
+      <c r="H6" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="85" t="s">
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="81" t="s">
+      <c r="H7" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="92"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="43">
         <v>1</v>
       </c>
@@ -1857,7 +1857,7 @@
       <c r="J9" s="40"/>
       <c r="K9" s="16"/>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="43"/>
       <c r="B10" s="45" t="s">
         <v>42</v>
@@ -1884,7 +1884,7 @@
       <c r="J10" s="44"/>
       <c r="K10" s="16"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="43"/>
       <c r="B11" s="45" t="s">
         <v>38</v>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="K11" s="16"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="43"/>
       <c r="B12" s="45" t="s">
         <v>52</v>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="K12" s="16"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="30"/>
       <c r="C13" s="27"/>
@@ -1947,7 +1947,7 @@
       <c r="R13" s="31"/>
       <c r="S13" s="31"/>
     </row>
-    <row r="14" spans="1:19" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="43">
         <v>2</v>
       </c>
@@ -1964,7 +1964,7 @@
       <c r="J14" s="40"/>
       <c r="K14" s="16"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="43"/>
       <c r="B15" s="45" t="s">
         <v>42</v>
@@ -1989,7 +1989,7 @@
       <c r="J15" s="44"/>
       <c r="K15" s="16"/>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="43"/>
       <c r="B16" s="45" t="s">
         <v>44</v>
@@ -2014,7 +2014,7 @@
       <c r="J16" s="44"/>
       <c r="K16" s="16"/>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="43"/>
       <c r="B17" s="45" t="s">
         <v>43</v>
@@ -2039,7 +2039,7 @@
       <c r="J17" s="44"/>
       <c r="K17" s="16"/>
     </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="43"/>
       <c r="B18" s="45" t="s">
         <v>65</v>
@@ -2063,7 +2063,7 @@
       <c r="J18" s="44"/>
       <c r="K18" s="16"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43"/>
       <c r="B19" s="45" t="s">
         <v>90</v>
@@ -2089,7 +2089,7 @@
       <c r="J19" s="44"/>
       <c r="K19" s="16"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43"/>
       <c r="B20" s="45" t="s">
         <v>91</v>
@@ -2115,7 +2115,7 @@
       <c r="J20" s="44"/>
       <c r="K20" s="16"/>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="43"/>
       <c r="B21" s="45" t="s">
         <v>92</v>
@@ -2141,7 +2141,7 @@
       <c r="J21" s="44"/>
       <c r="K21" s="16"/>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="43"/>
       <c r="B22" s="45" t="s">
         <v>38</v>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="K22" s="16"/>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="43"/>
       <c r="B23" s="45" t="s">
         <v>52</v>
@@ -2185,7 +2185,7 @@
       </c>
       <c r="K23" s="16"/>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="B24" s="30"/>
       <c r="C24" s="27"/>
@@ -2205,7 +2205,7 @@
       <c r="R24" s="31"/>
       <c r="S24" s="31"/>
     </row>
-    <row r="25" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="26">
         <v>3</v>
       </c>
@@ -2229,7 +2229,7 @@
       <c r="R25" s="31"/>
       <c r="S25" s="31"/>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="43"/>
       <c r="B26" s="45" t="s">
         <v>79</v>
@@ -2252,7 +2252,7 @@
       <c r="J26" s="44"/>
       <c r="K26" s="16"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="43"/>
       <c r="B27" s="45" t="s">
         <v>38</v>
@@ -2278,7 +2278,7 @@
       </c>
       <c r="K27" s="16"/>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="43"/>
       <c r="B28" s="45" t="s">
         <v>52</v>
@@ -2296,7 +2296,7 @@
       </c>
       <c r="K28" s="16"/>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="30"/>
       <c r="C29" s="27"/>
@@ -2316,7 +2316,7 @@
       <c r="R29" s="31"/>
       <c r="S29" s="31"/>
     </row>
-    <row r="30" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="26">
         <v>3</v>
       </c>
@@ -2340,7 +2340,7 @@
       <c r="R30" s="31"/>
       <c r="S30" s="31"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="43"/>
       <c r="B31" s="45" t="s">
         <v>79</v>
@@ -2363,7 +2363,7 @@
       <c r="J31" s="44"/>
       <c r="K31" s="16"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="43"/>
       <c r="B32" s="45" t="s">
         <v>38</v>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="K32" s="16"/>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="43"/>
       <c r="B33" s="45" t="s">
         <v>52</v>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="K33" s="16"/>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26"/>
       <c r="B34" s="30"/>
       <c r="C34" s="27"/>
@@ -2427,7 +2427,7 @@
       <c r="R34" s="31"/>
       <c r="S34" s="31"/>
     </row>
-    <row r="35" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="26">
         <v>3</v>
       </c>
@@ -2451,7 +2451,7 @@
       <c r="R35" s="31"/>
       <c r="S35" s="31"/>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="43"/>
       <c r="B36" s="45" t="s">
         <v>79</v>
@@ -2474,7 +2474,7 @@
       <c r="J36" s="44"/>
       <c r="K36" s="16"/>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="43"/>
       <c r="B37" s="45" t="s">
         <v>38</v>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="K37" s="16"/>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="43"/>
       <c r="B38" s="45" t="s">
         <v>52</v>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="K38" s="16"/>
     </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26"/>
       <c r="B39" s="30"/>
       <c r="C39" s="27"/>
@@ -2538,7 +2538,7 @@
       <c r="R39" s="31"/>
       <c r="S39" s="31"/>
     </row>
-    <row r="40" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="26">
         <v>3</v>
       </c>
@@ -2562,7 +2562,7 @@
       <c r="R40" s="31"/>
       <c r="S40" s="31"/>
     </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="43"/>
       <c r="B41" s="45" t="s">
         <v>79</v>
@@ -2585,7 +2585,7 @@
       <c r="J41" s="44"/>
       <c r="K41" s="16"/>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="43"/>
       <c r="B42" s="45" t="s">
         <v>38</v>
@@ -2611,7 +2611,7 @@
       </c>
       <c r="K42" s="16"/>
     </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="43"/>
       <c r="B43" s="45" t="s">
         <v>52</v>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="K43" s="16"/>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="26"/>
       <c r="B44" s="30"/>
       <c r="C44" s="27"/>
@@ -2649,7 +2649,7 @@
       <c r="R44" s="31"/>
       <c r="S44" s="31"/>
     </row>
-    <row r="45" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="64">
         <v>3</v>
       </c>
@@ -2673,7 +2673,7 @@
       <c r="R45" s="31"/>
       <c r="S45" s="31"/>
     </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="43"/>
       <c r="B46" s="45" t="s">
         <v>79</v>
@@ -2696,7 +2696,7 @@
       <c r="J46" s="44"/>
       <c r="K46" s="16"/>
     </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="43"/>
       <c r="B47" s="45" t="s">
         <v>38</v>
@@ -2722,7 +2722,7 @@
       </c>
       <c r="K47" s="16"/>
     </row>
-    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="43"/>
       <c r="B48" s="45" t="s">
         <v>52</v>
@@ -2740,7 +2740,7 @@
       </c>
       <c r="K48" s="16"/>
     </row>
-    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="26"/>
       <c r="B49" s="30"/>
       <c r="C49" s="27"/>
@@ -2760,7 +2760,7 @@
       <c r="R49" s="31"/>
       <c r="S49" s="31"/>
     </row>
-    <row r="50" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="64">
         <v>3</v>
       </c>
@@ -2784,7 +2784,7 @@
       <c r="R50" s="31"/>
       <c r="S50" s="31"/>
     </row>
-    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="43"/>
       <c r="B51" s="45" t="s">
         <v>79</v>
@@ -2807,7 +2807,7 @@
       <c r="J51" s="44"/>
       <c r="K51" s="16"/>
     </row>
-    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="43"/>
       <c r="B52" s="45" t="s">
         <v>38</v>
@@ -2833,7 +2833,7 @@
       </c>
       <c r="K52" s="16"/>
     </row>
-    <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="43"/>
       <c r="B53" s="45" t="s">
         <v>52</v>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="K53" s="16"/>
     </row>
-    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="26"/>
       <c r="B54" s="30"/>
       <c r="C54" s="27"/>
@@ -2871,7 +2871,7 @@
       <c r="R54" s="31"/>
       <c r="S54" s="31"/>
     </row>
-    <row r="55" spans="1:19" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="64">
         <v>3</v>
       </c>
@@ -2895,7 +2895,7 @@
       <c r="R55" s="31"/>
       <c r="S55" s="31"/>
     </row>
-    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="43"/>
       <c r="B56" s="45" t="s">
         <v>79</v>
@@ -2918,7 +2918,7 @@
       <c r="J56" s="44"/>
       <c r="K56" s="16"/>
     </row>
-    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="43"/>
       <c r="B57" s="45" t="s">
         <v>38</v>
@@ -2944,7 +2944,7 @@
       </c>
       <c r="K57" s="16"/>
     </row>
-    <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="43"/>
       <c r="B58" s="45" t="s">
         <v>52</v>
@@ -2962,7 +2962,7 @@
       </c>
       <c r="K58" s="16"/>
     </row>
-    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="26"/>
       <c r="B59" s="30"/>
       <c r="C59" s="27"/>
@@ -2982,7 +2982,7 @@
       <c r="R59" s="31"/>
       <c r="S59" s="31"/>
     </row>
-    <row r="60" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="64">
         <v>3</v>
       </c>
@@ -3006,7 +3006,7 @@
       <c r="R60" s="31"/>
       <c r="S60" s="31"/>
     </row>
-    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="43"/>
       <c r="B61" s="45" t="s">
         <v>79</v>
@@ -3029,7 +3029,7 @@
       <c r="J61" s="44"/>
       <c r="K61" s="16"/>
     </row>
-    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="43"/>
       <c r="B62" s="45" t="s">
         <v>38</v>
@@ -3055,7 +3055,7 @@
       </c>
       <c r="K62" s="16"/>
     </row>
-    <row r="63" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="43"/>
       <c r="B63" s="45" t="s">
         <v>52</v>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="K63" s="16"/>
     </row>
-    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="26"/>
       <c r="B64" s="30"/>
       <c r="C64" s="27"/>
@@ -3093,7 +3093,7 @@
       <c r="R64" s="31"/>
       <c r="S64" s="31"/>
     </row>
-    <row r="65" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="64">
         <v>3</v>
       </c>
@@ -3117,7 +3117,7 @@
       <c r="R65" s="31"/>
       <c r="S65" s="31"/>
     </row>
-    <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="43"/>
       <c r="B66" s="45" t="s">
         <v>79</v>
@@ -3140,7 +3140,7 @@
       <c r="J66" s="44"/>
       <c r="K66" s="16"/>
     </row>
-    <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="43"/>
       <c r="B67" s="45" t="s">
         <v>38</v>
@@ -3166,7 +3166,7 @@
       </c>
       <c r="K67" s="16"/>
     </row>
-    <row r="68" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="43"/>
       <c r="B68" s="45" t="s">
         <v>52</v>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="K68" s="16"/>
     </row>
-    <row r="69" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="26"/>
       <c r="B69" s="30"/>
       <c r="C69" s="27"/>
@@ -3204,7 +3204,7 @@
       <c r="R69" s="31"/>
       <c r="S69" s="31"/>
     </row>
-    <row r="70" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="64">
         <v>3</v>
       </c>
@@ -3228,7 +3228,7 @@
       <c r="R70" s="31"/>
       <c r="S70" s="31"/>
     </row>
-    <row r="71" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="43"/>
       <c r="B71" s="45" t="s">
         <v>79</v>
@@ -3251,7 +3251,7 @@
       <c r="J71" s="44"/>
       <c r="K71" s="16"/>
     </row>
-    <row r="72" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="43"/>
       <c r="B72" s="45" t="s">
         <v>38</v>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="K72" s="16"/>
     </row>
-    <row r="73" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="43"/>
       <c r="B73" s="45" t="s">
         <v>52</v>
@@ -3295,7 +3295,7 @@
       </c>
       <c r="K73" s="16"/>
     </row>
-    <row r="74" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="26"/>
       <c r="B74" s="30"/>
       <c r="C74" s="27"/>
@@ -3315,7 +3315,7 @@
       <c r="R74" s="31"/>
       <c r="S74" s="31"/>
     </row>
-    <row r="75" spans="1:19" ht="30" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="26">
         <v>3</v>
       </c>
@@ -3339,7 +3339,7 @@
       <c r="R75" s="31"/>
       <c r="S75" s="31"/>
     </row>
-    <row r="76" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="43"/>
       <c r="B76" s="45" t="s">
         <v>54</v>
@@ -3363,7 +3363,7 @@
       <c r="J76" s="44"/>
       <c r="K76" s="16"/>
     </row>
-    <row r="77" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="43"/>
       <c r="B77" s="45" t="s">
         <v>38</v>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="K77" s="16"/>
     </row>
-    <row r="78" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="43"/>
       <c r="B78" s="45" t="s">
         <v>52</v>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="K78" s="16"/>
     </row>
-    <row r="79" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="43"/>
       <c r="B79" s="45"/>
       <c r="C79" s="46"/>
@@ -3419,7 +3419,7 @@
       <c r="J79" s="40"/>
       <c r="K79" s="16"/>
     </row>
-    <row r="80" spans="1:19" ht="30" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="43">
         <v>4</v>
       </c>
@@ -3436,7 +3436,7 @@
       <c r="J80" s="40"/>
       <c r="K80" s="16"/>
     </row>
-    <row r="81" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="43"/>
       <c r="B81" s="45" t="s">
         <v>54</v>
@@ -3461,7 +3461,7 @@
       <c r="J81" s="44"/>
       <c r="K81" s="16"/>
     </row>
-    <row r="82" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="43"/>
       <c r="B82" s="45" t="s">
         <v>55</v>
@@ -3486,7 +3486,7 @@
       <c r="J82" s="44"/>
       <c r="K82" s="16"/>
     </row>
-    <row r="83" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="43"/>
       <c r="B83" s="45" t="s">
         <v>38</v>
@@ -3511,7 +3511,7 @@
       </c>
       <c r="K83" s="16"/>
     </row>
-    <row r="84" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="43"/>
       <c r="B84" s="45" t="s">
         <v>52</v>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="K84" s="16"/>
     </row>
-    <row r="85" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="43"/>
       <c r="B85" s="45"/>
       <c r="C85" s="46"/>
@@ -3542,7 +3542,7 @@
       <c r="J85" s="40"/>
       <c r="K85" s="16"/>
     </row>
-    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="43">
         <v>5</v>
       </c>
@@ -3559,7 +3559,7 @@
       <c r="J86" s="40"/>
       <c r="K86" s="16"/>
     </row>
-    <row r="87" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="43"/>
       <c r="B87" s="45" t="s">
         <v>54</v>
@@ -3584,7 +3584,7 @@
       <c r="J87" s="44"/>
       <c r="K87" s="16"/>
     </row>
-    <row r="88" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="43"/>
       <c r="B88" s="45" t="s">
         <v>38</v>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="K88" s="16"/>
     </row>
-    <row r="89" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="43"/>
       <c r="B89" s="45" t="s">
         <v>52</v>
@@ -3627,7 +3627,7 @@
       </c>
       <c r="K89" s="16"/>
     </row>
-    <row r="90" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="43"/>
       <c r="B90" s="45"/>
       <c r="C90" s="46"/>
@@ -3640,7 +3640,7 @@
       <c r="J90" s="40"/>
       <c r="K90" s="16"/>
     </row>
-    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="58">
         <v>6</v>
       </c>
@@ -3657,7 +3657,7 @@
       <c r="J91" s="40"/>
       <c r="K91" s="16"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="43"/>
       <c r="B92" s="45" t="str">
         <f>B82</f>
@@ -3684,7 +3684,7 @@
       <c r="J92" s="9"/>
       <c r="K92" s="16"/>
     </row>
-    <row r="93" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="43"/>
       <c r="B93" s="45" t="s">
         <v>38</v>
@@ -3710,7 +3710,7 @@
       </c>
       <c r="K93" s="16"/>
     </row>
-    <row r="94" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="43"/>
       <c r="B94" s="45" t="s">
         <v>52</v>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="K94" s="16"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="43"/>
       <c r="B95" s="45"/>
       <c r="C95" s="46"/>
@@ -3741,7 +3741,7 @@
       <c r="J95" s="40"/>
       <c r="K95" s="16"/>
     </row>
-    <row r="96" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="58">
         <v>7</v>
       </c>
@@ -3758,7 +3758,7 @@
       <c r="J96" s="40"/>
       <c r="K96" s="16"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="43"/>
       <c r="B97" s="45" t="s">
         <v>60</v>
@@ -3784,7 +3784,7 @@
       <c r="J97" s="9"/>
       <c r="K97" s="16"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="43"/>
       <c r="B98" s="45" t="s">
         <v>61</v>
@@ -3808,7 +3808,7 @@
       <c r="J98" s="9"/>
       <c r="K98" s="16"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="43"/>
       <c r="B99" s="45"/>
       <c r="C99" s="46">
@@ -3830,7 +3830,7 @@
       <c r="J99" s="9"/>
       <c r="K99" s="16"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="43"/>
       <c r="B100" s="45"/>
       <c r="C100" s="46">
@@ -3853,7 +3853,7 @@
       <c r="J100" s="9"/>
       <c r="K100" s="16"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="43"/>
       <c r="B101" s="45"/>
       <c r="C101" s="46">
@@ -3875,7 +3875,7 @@
       <c r="J101" s="9"/>
       <c r="K101" s="16"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="43"/>
       <c r="B102" s="45" t="s">
         <v>76</v>
@@ -3901,7 +3901,7 @@
       <c r="J102" s="9"/>
       <c r="K102" s="16"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="43"/>
       <c r="B103" s="45" t="s">
         <v>77</v>
@@ -3927,7 +3927,7 @@
       <c r="J103" s="9"/>
       <c r="K103" s="16"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="43"/>
       <c r="B104" s="45"/>
       <c r="C104" s="46">
@@ -3951,7 +3951,7 @@
       <c r="J104" s="9"/>
       <c r="K104" s="16"/>
     </row>
-    <row r="105" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="43"/>
       <c r="B105" s="45" t="s">
         <v>38</v>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="K105" s="16"/>
     </row>
-    <row r="106" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="43"/>
       <c r="B106" s="45" t="s">
         <v>52</v>
@@ -3994,7 +3994,7 @@
       </c>
       <c r="K106" s="16"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="43"/>
       <c r="B107" s="45"/>
       <c r="C107" s="46"/>
@@ -4007,7 +4007,7 @@
       <c r="J107" s="40"/>
       <c r="K107" s="16"/>
     </row>
-    <row r="108" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="43">
         <v>8</v>
       </c>
@@ -4024,7 +4024,7 @@
       <c r="J108" s="40"/>
       <c r="K108" s="16"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="43"/>
       <c r="B109" s="45" t="s">
         <v>63</v>
@@ -4047,7 +4047,7 @@
       <c r="J109" s="9"/>
       <c r="K109" s="16"/>
     </row>
-    <row r="110" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="43"/>
       <c r="B110" s="45" t="s">
         <v>38</v>
@@ -4072,7 +4072,7 @@
       </c>
       <c r="K110" s="16"/>
     </row>
-    <row r="111" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="43"/>
       <c r="B111" s="45" t="s">
         <v>52</v>
@@ -4090,7 +4090,7 @@
       </c>
       <c r="K111" s="16"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="43"/>
       <c r="B112" s="45"/>
       <c r="C112" s="46"/>
@@ -4103,7 +4103,7 @@
       <c r="J112" s="40"/>
       <c r="K112" s="16"/>
     </row>
-    <row r="113" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="43">
         <v>9</v>
       </c>
@@ -4120,7 +4120,7 @@
       <c r="J113" s="40"/>
       <c r="K113" s="16"/>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="43"/>
       <c r="B114" s="45" t="s">
         <v>63</v>
@@ -4143,7 +4143,7 @@
       <c r="J114" s="9"/>
       <c r="K114" s="16"/>
     </row>
-    <row r="115" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="43"/>
       <c r="B115" s="45" t="s">
         <v>38</v>
@@ -4168,7 +4168,7 @@
       </c>
       <c r="K115" s="16"/>
     </row>
-    <row r="116" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="43"/>
       <c r="B116" s="45" t="s">
         <v>52</v>
@@ -4186,7 +4186,7 @@
       </c>
       <c r="K116" s="16"/>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="43"/>
       <c r="B117" s="45"/>
       <c r="C117" s="46"/>
@@ -4199,7 +4199,7 @@
       <c r="J117" s="40"/>
       <c r="K117" s="16"/>
     </row>
-    <row r="118" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="43">
         <v>10</v>
       </c>
@@ -4216,7 +4216,7 @@
       <c r="J118" s="40"/>
       <c r="K118" s="5"/>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="43"/>
       <c r="B119" s="56" t="s">
         <v>67</v>
@@ -4244,7 +4244,7 @@
       <c r="J119" s="40"/>
       <c r="K119" s="5"/>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="43"/>
       <c r="B120" s="56"/>
       <c r="C120" s="53">
@@ -4269,7 +4269,7 @@
       <c r="J120" s="40"/>
       <c r="K120" s="5"/>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="43"/>
       <c r="B121" s="56" t="s">
         <v>68</v>
@@ -4296,7 +4296,7 @@
       <c r="J121" s="40"/>
       <c r="K121" s="5"/>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="43"/>
       <c r="B122" s="56"/>
       <c r="C122" s="53">
@@ -4322,7 +4322,7 @@
       <c r="J122" s="40"/>
       <c r="K122" s="5"/>
     </row>
-    <row r="123" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="43"/>
       <c r="B123" s="56" t="s">
         <v>38</v>
@@ -4348,7 +4348,7 @@
       </c>
       <c r="K123" s="5"/>
     </row>
-    <row r="124" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="43"/>
       <c r="B124" s="56" t="s">
         <v>52</v>
@@ -4366,7 +4366,7 @@
       </c>
       <c r="K124" s="5"/>
     </row>
-    <row r="125" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="43"/>
       <c r="B125" s="56"/>
       <c r="C125" s="53"/>
@@ -4379,7 +4379,7 @@
       <c r="J125" s="61"/>
       <c r="K125" s="5"/>
     </row>
-    <row r="126" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A126" s="43">
         <v>11</v>
       </c>
@@ -4397,7 +4397,7 @@
       <c r="K126" s="5"/>
       <c r="M126" s="63"/>
     </row>
-    <row r="127" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="43"/>
       <c r="B127" s="56" t="s">
         <v>70</v>
@@ -4423,7 +4423,7 @@
       <c r="J127" s="40"/>
       <c r="K127" s="5"/>
     </row>
-    <row r="128" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="43"/>
       <c r="B128" s="56" t="s">
         <v>38</v>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="K128" s="5"/>
     </row>
-    <row r="129" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="43"/>
       <c r="B129" s="56" t="s">
         <v>52</v>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="K129" s="5"/>
     </row>
-    <row r="130" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="43"/>
       <c r="B130" s="52"/>
       <c r="C130" s="53"/>
@@ -4481,7 +4481,7 @@
       <c r="K130" s="5"/>
       <c r="M130" s="63"/>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="43">
         <v>12</v>
       </c>
@@ -4498,7 +4498,7 @@
       <c r="J131" s="40"/>
       <c r="K131" s="5"/>
     </row>
-    <row r="132" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="43"/>
       <c r="B132" s="56" t="s">
         <v>70</v>
@@ -4524,7 +4524,7 @@
       <c r="J132" s="40"/>
       <c r="K132" s="5"/>
     </row>
-    <row r="133" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="43"/>
       <c r="B133" s="56" t="s">
         <v>38</v>
@@ -4550,7 +4550,7 @@
       </c>
       <c r="K133" s="5"/>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="43"/>
       <c r="B134" s="62"/>
       <c r="C134" s="53"/>
@@ -4563,7 +4563,7 @@
       <c r="J134" s="40"/>
       <c r="K134" s="5"/>
     </row>
-    <row r="135" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="43">
         <v>13</v>
       </c>
@@ -4580,7 +4580,7 @@
       <c r="J135" s="40"/>
       <c r="K135" s="5"/>
     </row>
-    <row r="136" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="43"/>
       <c r="B136" s="56" t="s">
         <v>72</v>
@@ -4606,7 +4606,7 @@
       <c r="J136" s="40"/>
       <c r="K136" s="5"/>
     </row>
-    <row r="137" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="43"/>
       <c r="B137" s="56" t="s">
         <v>38</v>
@@ -4632,7 +4632,7 @@
       </c>
       <c r="K137" s="5"/>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="43"/>
       <c r="B138" s="62"/>
       <c r="C138" s="53"/>
@@ -4645,7 +4645,7 @@
       <c r="J138" s="40"/>
       <c r="K138" s="5"/>
     </row>
-    <row r="139" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A139" s="43">
         <v>14</v>
       </c>
@@ -4662,7 +4662,7 @@
       <c r="J139" s="40"/>
       <c r="K139" s="5"/>
     </row>
-    <row r="140" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="43"/>
       <c r="B140" s="56" t="s">
         <v>74</v>
@@ -4688,32 +4688,32 @@
       <c r="J140" s="40"/>
       <c r="K140" s="5"/>
     </row>
-    <row r="141" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="43"/>
-      <c r="B141" s="93" t="s">
+      <c r="B141" s="70" t="s">
         <v>96</v>
       </c>
-      <c r="C141" s="90">
+      <c r="C141" s="67">
         <v>4</v>
       </c>
-      <c r="D141" s="91">
+      <c r="D141" s="68">
         <f>0.6</f>
         <v>0.6</v>
       </c>
-      <c r="E141" s="91"/>
-      <c r="F141" s="91">
+      <c r="E141" s="68"/>
+      <c r="F141" s="68">
         <v>0.6</v>
       </c>
-      <c r="G141" s="91">
-        <f>PRODUCT(C141:F141)</f>
-        <v>1.44</v>
+      <c r="G141" s="68">
+        <f>0*PRODUCT(C141:F141)</f>
+        <v>0</v>
       </c>
       <c r="H141" s="57"/>
       <c r="I141" s="57"/>
       <c r="J141" s="40"/>
       <c r="K141" s="5"/>
     </row>
-    <row r="142" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="43"/>
       <c r="B142" s="56" t="s">
         <v>38</v>
@@ -4724,7 +4724,7 @@
       <c r="F142" s="54"/>
       <c r="G142" s="55">
         <f>SUM(G140:G141)</f>
-        <v>1.9456115855877232</v>
+        <v>0.50561158558772312</v>
       </c>
       <c r="H142" s="55" t="s">
         <v>41</v>
@@ -4735,11 +4735,11 @@
       </c>
       <c r="J142" s="61">
         <f>G142*I142</f>
-        <v>117717.82476197125</v>
+        <v>30591.66406631907</v>
       </c>
       <c r="K142" s="5"/>
     </row>
-    <row r="143" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="43"/>
       <c r="B143" s="56" t="s">
         <v>52</v>
@@ -4753,11 +4753,11 @@
       <c r="I143" s="60"/>
       <c r="J143" s="61">
         <f>0.13*G142*(9888.94/0.92)</f>
-        <v>2718.7007720800452</v>
+        <v>706.51645903656697</v>
       </c>
       <c r="K143" s="5"/>
     </row>
-    <row r="144" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="43"/>
       <c r="B144" s="56"/>
       <c r="C144" s="53"/>
@@ -4771,253 +4771,253 @@
       <c r="K144" s="5"/>
       <c r="M144" s="63"/>
     </row>
-    <row r="145" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A145" s="88">
+    <row r="145" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A145" s="65">
         <v>15</v>
       </c>
-      <c r="B145" s="89" t="s">
+      <c r="B145" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="C145" s="90"/>
-      <c r="D145" s="91"/>
-      <c r="E145" s="91"/>
-      <c r="F145" s="91"/>
-      <c r="G145" s="91"/>
-      <c r="H145" s="91"/>
-      <c r="I145" s="91"/>
-      <c r="J145" s="92"/>
+      <c r="C145" s="67"/>
+      <c r="D145" s="68"/>
+      <c r="E145" s="68"/>
+      <c r="F145" s="68"/>
+      <c r="G145" s="68"/>
+      <c r="H145" s="68"/>
+      <c r="I145" s="68"/>
+      <c r="J145" s="69"/>
       <c r="K145" s="5"/>
       <c r="M145" s="63"/>
     </row>
-    <row r="146" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="88"/>
-      <c r="B146" s="93" t="s">
+    <row r="146" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="65"/>
+      <c r="B146" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="C146" s="90">
+      <c r="C146" s="67">
         <v>4</v>
       </c>
-      <c r="D146" s="91">
+      <c r="D146" s="68">
         <f>(14.75+5.17)/2/3.281</f>
         <v>3.0356598597988418</v>
       </c>
-      <c r="E146" s="91">
+      <c r="E146" s="68">
         <f>5.5/3.281</f>
         <v>1.6763181956720512</v>
       </c>
-      <c r="F146" s="91"/>
-      <c r="G146" s="91">
+      <c r="F146" s="68"/>
+      <c r="G146" s="68">
         <f>PRODUCT(C146:F146)</f>
         <v>20.354927435408264</v>
       </c>
-      <c r="H146" s="91"/>
-      <c r="I146" s="91"/>
-      <c r="J146" s="92"/>
+      <c r="H146" s="68"/>
+      <c r="I146" s="68"/>
+      <c r="J146" s="69"/>
       <c r="K146" s="5"/>
     </row>
-    <row r="147" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="88"/>
-      <c r="B147" s="93" t="s">
+    <row r="147" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="65"/>
+      <c r="B147" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="C147" s="90">
+      <c r="C147" s="67">
         <v>4</v>
       </c>
-      <c r="D147" s="91">
+      <c r="D147" s="68">
         <f>(10.75+1.5)/2/3.281</f>
         <v>1.8668088997256933</v>
       </c>
-      <c r="E147" s="91">
+      <c r="E147" s="68">
         <f>4.5/3.281</f>
         <v>1.3715330691862238</v>
       </c>
-      <c r="F147" s="91"/>
-      <c r="G147" s="91">
+      <c r="F147" s="68"/>
+      <c r="G147" s="68">
         <f>PRODUCT(C147:F147)</f>
         <v>10.241560559299749</v>
       </c>
-      <c r="H147" s="91"/>
-      <c r="I147" s="91"/>
-      <c r="J147" s="92"/>
+      <c r="H147" s="68"/>
+      <c r="I147" s="68"/>
+      <c r="J147" s="69"/>
       <c r="K147" s="5"/>
     </row>
-    <row r="148" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="88"/>
-      <c r="B148" s="93" t="s">
+    <row r="148" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="65"/>
+      <c r="B148" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="C148" s="90"/>
-      <c r="D148" s="91"/>
-      <c r="E148" s="91"/>
-      <c r="F148" s="91"/>
-      <c r="G148" s="94">
-        <f>SUM(G146:G147)</f>
-        <v>30.596487994708014</v>
-      </c>
-      <c r="H148" s="94" t="s">
+      <c r="C148" s="67"/>
+      <c r="D148" s="68"/>
+      <c r="E148" s="68"/>
+      <c r="F148" s="68"/>
+      <c r="G148" s="71">
+        <f>0*SUM(G146:G147)</f>
+        <v>0</v>
+      </c>
+      <c r="H148" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="I148" s="95">
+      <c r="I148" s="72">
         <f>1132.13/1.15</f>
         <v>984.46086956521754</v>
       </c>
-      <c r="J148" s="96">
+      <c r="J148" s="73">
         <f>G148*I148</f>
-        <v>30121.04517691199</v>
+        <v>0</v>
       </c>
       <c r="K148" s="5"/>
     </row>
-    <row r="149" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="88"/>
-      <c r="B149" s="93" t="s">
+    <row r="149" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="65"/>
+      <c r="B149" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="C149" s="90"/>
-      <c r="D149" s="91"/>
-      <c r="E149" s="91"/>
-      <c r="F149" s="91"/>
-      <c r="G149" s="94"/>
-      <c r="H149" s="94"/>
-      <c r="I149" s="95"/>
-      <c r="J149" s="96">
+      <c r="C149" s="67"/>
+      <c r="D149" s="68"/>
+      <c r="E149" s="68"/>
+      <c r="F149" s="68"/>
+      <c r="G149" s="71"/>
+      <c r="H149" s="71"/>
+      <c r="I149" s="72"/>
+      <c r="J149" s="73">
         <f>0.13*G148*(2795.1/10)</f>
-        <v>1111.7631667221087</v>
+        <v>0</v>
       </c>
       <c r="K149" s="5"/>
     </row>
-    <row r="150" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A150" s="88"/>
-      <c r="B150" s="97"/>
-      <c r="C150" s="90"/>
-      <c r="D150" s="91"/>
-      <c r="E150" s="91"/>
-      <c r="F150" s="91"/>
-      <c r="G150" s="91"/>
-      <c r="H150" s="91"/>
-      <c r="I150" s="91"/>
-      <c r="J150" s="92"/>
+    <row r="150" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A150" s="65"/>
+      <c r="B150" s="74"/>
+      <c r="C150" s="67"/>
+      <c r="D150" s="68"/>
+      <c r="E150" s="68"/>
+      <c r="F150" s="68"/>
+      <c r="G150" s="68"/>
+      <c r="H150" s="68"/>
+      <c r="I150" s="68"/>
+      <c r="J150" s="69"/>
       <c r="K150" s="5"/>
       <c r="M150" s="63"/>
     </row>
-    <row r="151" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A151" s="88">
+    <row r="151" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A151" s="65">
         <v>16</v>
       </c>
-      <c r="B151" s="98" t="s">
+      <c r="B151" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="C151" s="90"/>
-      <c r="D151" s="91"/>
-      <c r="E151" s="91"/>
-      <c r="F151" s="91"/>
-      <c r="G151" s="91"/>
-      <c r="H151" s="91"/>
-      <c r="I151" s="91"/>
-      <c r="J151" s="92"/>
+      <c r="C151" s="67"/>
+      <c r="D151" s="68"/>
+      <c r="E151" s="68"/>
+      <c r="F151" s="68"/>
+      <c r="G151" s="68"/>
+      <c r="H151" s="68"/>
+      <c r="I151" s="68"/>
+      <c r="J151" s="69"/>
       <c r="K151" s="5"/>
       <c r="M151" s="63"/>
     </row>
-    <row r="152" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="88"/>
-      <c r="B152" s="93" t="str">
-        <f>B146</f>
+    <row r="152" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="65"/>
+      <c r="B152" s="70" t="str">
+        <f t="shared" ref="B152:E153" si="12">B146</f>
         <v>-First floor inclined roof</v>
       </c>
-      <c r="C152" s="90">
-        <f>C146</f>
+      <c r="C152" s="67">
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
-      <c r="D152" s="91">
-        <f>D146</f>
+      <c r="D152" s="68">
+        <f t="shared" si="12"/>
         <v>3.0356598597988418</v>
       </c>
-      <c r="E152" s="91">
-        <f>E146</f>
+      <c r="E152" s="68">
+        <f t="shared" si="12"/>
         <v>1.6763181956720512</v>
       </c>
-      <c r="F152" s="91"/>
-      <c r="G152" s="91">
+      <c r="F152" s="68"/>
+      <c r="G152" s="68">
         <f>PRODUCT(C152:F152)</f>
         <v>20.354927435408264</v>
       </c>
-      <c r="H152" s="91"/>
-      <c r="I152" s="91"/>
-      <c r="J152" s="92"/>
+      <c r="H152" s="68"/>
+      <c r="I152" s="68"/>
+      <c r="J152" s="69"/>
       <c r="K152" s="5"/>
     </row>
-    <row r="153" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="88"/>
-      <c r="B153" s="93" t="str">
-        <f>B147</f>
+    <row r="153" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="65"/>
+      <c r="B153" s="70" t="str">
+        <f t="shared" si="12"/>
         <v>-Second floor inclined roof</v>
       </c>
-      <c r="C153" s="90">
-        <f>C147</f>
+      <c r="C153" s="67">
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
-      <c r="D153" s="91">
-        <f>D147</f>
+      <c r="D153" s="68">
+        <f t="shared" si="12"/>
         <v>1.8668088997256933</v>
       </c>
-      <c r="E153" s="91">
-        <f>E147</f>
+      <c r="E153" s="68">
+        <f t="shared" si="12"/>
         <v>1.3715330691862238</v>
       </c>
-      <c r="F153" s="91"/>
-      <c r="G153" s="91">
+      <c r="F153" s="68"/>
+      <c r="G153" s="68">
         <f>PRODUCT(C153:F153)</f>
         <v>10.241560559299749</v>
       </c>
-      <c r="H153" s="91"/>
-      <c r="I153" s="91"/>
-      <c r="J153" s="92"/>
+      <c r="H153" s="68"/>
+      <c r="I153" s="68"/>
+      <c r="J153" s="69"/>
       <c r="K153" s="5"/>
     </row>
-    <row r="154" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="88"/>
-      <c r="B154" s="93" t="s">
+    <row r="154" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="65"/>
+      <c r="B154" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="C154" s="90"/>
-      <c r="D154" s="91"/>
-      <c r="E154" s="91"/>
-      <c r="F154" s="91"/>
-      <c r="G154" s="94">
-        <f>SUM(G152:G153)</f>
-        <v>30.596487994708014</v>
-      </c>
-      <c r="H154" s="94" t="s">
+      <c r="C154" s="67"/>
+      <c r="D154" s="68"/>
+      <c r="E154" s="68"/>
+      <c r="F154" s="68"/>
+      <c r="G154" s="71">
+        <f>0*SUM(G152:G153)</f>
+        <v>0</v>
+      </c>
+      <c r="H154" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="I154" s="95">
+      <c r="I154" s="72">
         <f>4842.49/1.15</f>
         <v>4210.8608695652174</v>
       </c>
-      <c r="J154" s="96">
+      <c r="J154" s="73">
         <f>G154*I154</f>
-        <v>128837.55404303792</v>
+        <v>0</v>
       </c>
       <c r="K154" s="5"/>
     </row>
-    <row r="155" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="88"/>
-      <c r="B155" s="93" t="s">
+    <row r="155" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="65"/>
+      <c r="B155" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="C155" s="90"/>
-      <c r="D155" s="91"/>
-      <c r="E155" s="91"/>
-      <c r="F155" s="91"/>
-      <c r="G155" s="94"/>
-      <c r="H155" s="94"/>
-      <c r="I155" s="95"/>
-      <c r="J155" s="96">
+      <c r="C155" s="67"/>
+      <c r="D155" s="68"/>
+      <c r="E155" s="68"/>
+      <c r="F155" s="68"/>
+      <c r="G155" s="71"/>
+      <c r="H155" s="71"/>
+      <c r="I155" s="72"/>
+      <c r="J155" s="73">
         <f>0.13*G154*(315405.75/100)</f>
-        <v>12545.400716337939</v>
+        <v>0</v>
       </c>
       <c r="K155" s="5"/>
     </row>
-    <row r="156" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="43"/>
       <c r="B156" s="52"/>
       <c r="C156" s="53"/>
@@ -5031,7 +5031,7 @@
       <c r="K156" s="5"/>
       <c r="M156" s="63"/>
     </row>
-    <row r="157" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="43"/>
       <c r="B157" s="56"/>
       <c r="C157" s="53"/>
@@ -5045,7 +5045,7 @@
       <c r="K157" s="5"/>
       <c r="M157" s="63"/>
     </row>
-    <row r="158" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="43"/>
       <c r="B158" s="56"/>
       <c r="C158" s="53"/>
@@ -5059,7 +5059,7 @@
       <c r="K158" s="5"/>
       <c r="M158" s="63"/>
     </row>
-    <row r="159" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="43"/>
       <c r="B159" s="56"/>
       <c r="C159" s="53"/>
@@ -5073,7 +5073,7 @@
       <c r="K159" s="5"/>
       <c r="M159" s="63"/>
     </row>
-    <row r="160" spans="1:19" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A160" s="26">
         <v>15</v>
       </c>
@@ -5109,7 +5109,7 @@
       <c r="R160" s="31"/>
       <c r="S160" s="31"/>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" s="43"/>
       <c r="B161" s="45"/>
       <c r="C161" s="46"/>
@@ -5122,7 +5122,7 @@
       <c r="J161" s="44"/>
       <c r="K161" s="16"/>
     </row>
-    <row r="162" spans="1:20" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A162" s="26">
         <v>16</v>
       </c>
@@ -5136,7 +5136,7 @@
       <c r="E162" s="29"/>
       <c r="F162" s="29"/>
       <c r="G162" s="44">
-        <f t="shared" ref="G162" si="12">PRODUCT(C162:F162)</f>
+        <f t="shared" ref="G162" si="13">PRODUCT(C162:F162)</f>
         <v>1</v>
       </c>
       <c r="H162" s="38" t="s">
@@ -5159,7 +5159,7 @@
       <c r="S162" s="18"/>
       <c r="T162" s="18"/>
     </row>
-    <row r="163" spans="1:20" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A163" s="26"/>
       <c r="B163" s="30"/>
       <c r="C163" s="27"/>
@@ -5180,7 +5180,7 @@
       <c r="S163" s="18"/>
       <c r="T163" s="18"/>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" s="43"/>
       <c r="B164" s="50" t="s">
         <v>15</v>
@@ -5194,19 +5194,19 @@
       <c r="I164" s="44"/>
       <c r="J164" s="44">
         <f>SUM(J10:J162)</f>
-        <v>899525.9405074158</v>
+        <v>637771.83239571028</v>
       </c>
       <c r="K164" s="16"/>
     </row>
-    <row r="166" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B166" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C166" s="79">
+      <c r="C166" s="90">
         <f>J164</f>
-        <v>899525.9405074158</v>
-      </c>
-      <c r="D166" s="80"/>
+        <v>637771.83239571028</v>
+      </c>
+      <c r="D166" s="91"/>
       <c r="E166" s="14">
         <v>100</v>
       </c>
@@ -5217,66 +5217,66 @@
       <c r="J166" s="21"/>
       <c r="K166" s="22"/>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B167" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C167" s="86">
+      <c r="C167" s="97">
         <v>1000000</v>
       </c>
-      <c r="D167" s="87"/>
+      <c r="D167" s="98"/>
       <c r="E167" s="14"/>
     </row>
-    <row r="168" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B168" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C168" s="86">
+      <c r="C168" s="97">
         <f>C167-C170-C171</f>
         <v>950000</v>
       </c>
-      <c r="D168" s="87"/>
+      <c r="D168" s="98"/>
       <c r="E168" s="14">
         <f>C168/C166*100</f>
-        <v>105.61118442722311</v>
-      </c>
-    </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.3">
+        <v>148.95609240556195</v>
+      </c>
+    </row>
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B169" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C169" s="78">
+      <c r="C169" s="89">
         <f>C166-C168</f>
-        <v>-50474.059492584202</v>
-      </c>
-      <c r="D169" s="78"/>
+        <v>-312228.16760428972</v>
+      </c>
+      <c r="D169" s="89"/>
       <c r="E169" s="14">
         <f>100-E168</f>
-        <v>-5.6111844272231082</v>
-      </c>
-    </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.3">
+        <v>-48.956092405561947</v>
+      </c>
+    </row>
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B170" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C170" s="79">
+      <c r="C170" s="90">
         <f>C167*0.03</f>
         <v>30000</v>
       </c>
-      <c r="D170" s="80"/>
+      <c r="D170" s="91"/>
       <c r="E170" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B171" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C171" s="79">
+      <c r="C171" s="90">
         <f>C167*0.02</f>
         <v>20000</v>
       </c>
-      <c r="D171" s="80"/>
+      <c r="D171" s="91"/>
       <c r="E171" s="14">
         <v>2</v>
       </c>

</xml_diff>